<commit_message>
dual footprint for serial eprom
</commit_message>
<xml_diff>
--- a/BOM/Aries parts list rev 5.xlsx
+++ b/BOM/Aries parts list rev 5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C047F6-A208-4037-BAC2-E6CEA33DB539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD225C-F846-44E3-A1D2-4AF126729B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,9 +324,6 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>2.1mm 12V power</t>
-  </si>
-  <si>
     <t>Inductor windings:</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
   </si>
   <si>
     <t>616-3400</t>
-  </si>
-  <si>
-    <t>448-376</t>
   </si>
   <si>
     <t>654-5818</t>
@@ -616,6 +610,12 @@
   </si>
   <si>
     <t>MF-MSMF110_24X-2</t>
+  </si>
+  <si>
+    <t>MKDSP 1.5/ 2-5.08</t>
+  </si>
+  <si>
+    <t>651-1730120</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -1244,16 +1244,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1298,13 +1298,13 @@
         <v>22</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
@@ -1320,7 +1320,7 @@
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
@@ -1330,7 +1330,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>18</v>
@@ -1339,7 +1339,7 @@
         <v>85</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -1348,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
@@ -1364,7 +1364,7 @@
         <v>52</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>21</v>
@@ -1386,7 +1386,7 @@
         <v>21</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
@@ -1434,7 +1434,7 @@
         <v>21</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1482,7 +1482,7 @@
         <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1498,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>21</v>
@@ -1556,7 +1556,7 @@
         <v>5</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>21</v>
@@ -1572,7 +1572,7 @@
         <v>5</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>21</v>
@@ -1588,16 +1588,16 @@
         <v>6</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F28" s="5"/>
     </row>
@@ -1612,7 +1612,7 @@
         <v>37</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1622,13 +1622,13 @@
         <v>10</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1644,7 +1644,7 @@
         <v>37</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1660,7 +1660,7 @@
         <v>37</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1670,13 +1670,13 @@
         <v>2</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1693,7 +1693,7 @@
         <v>37</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1710,7 +1710,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1726,13 +1726,13 @@
         <v>90</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G36" s="9"/>
     </row>
@@ -1741,7 +1741,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>81</v>
@@ -1779,7 +1779,7 @@
         <v>81</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1789,7 +1789,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>60</v>
@@ -1807,13 +1807,13 @@
         <v>2</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>60</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1830,7 +1830,7 @@
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>87</v>
@@ -1841,16 +1841,16 @@
         <v>2</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F43" s="5"/>
     </row>
@@ -1865,10 +1865,10 @@
         <v>93</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>117</v>
+        <v>190</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1927,13 +1927,13 @@
         <v>2</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1943,13 +1943,13 @@
         <v>1</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1959,7 +1959,7 @@
         <v>3</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>93</v>
@@ -1977,123 +1977,123 @@
         <v>1</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C59" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>139</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" t="s">
         <v>141</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C64" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2101,15 +2101,15 @@
     </row>
     <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -2207,10 +2207,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
@@ -2224,11 +2224,11 @@
         <v>67</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -2317,7 +2317,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1</v>
@@ -2326,7 +2326,7 @@
         <v>75</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -2335,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -2351,20 +2351,20 @@
         <v>1</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1"/>
     </row>

</xml_diff>

<commit_message>
TRX relay back to G6A, minor changes
</commit_message>
<xml_diff>
--- a/BOM/Aries parts list rev 5.xlsx
+++ b/BOM/Aries parts list rev 5.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CD225C-F846-44E3-A1D2-4AF126729B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CDC2C3-E38F-450A-891A-170FB75D47EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="194">
   <si>
     <t>RL1-RL17</t>
   </si>
@@ -616,6 +616,15 @@
   </si>
   <si>
     <t>651-1730120</t>
+  </si>
+  <si>
+    <t>K18</t>
+  </si>
+  <si>
+    <t>G6A-274P</t>
+  </si>
+  <si>
+    <t>653-G6A-274P40-DC12</t>
   </si>
 </sst>
 </file>
@@ -748,13 +757,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1118,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1172,52 +1181,52 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>4</v>
+        <v>191</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>7</v>
+        <v>192</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>43</v>
+        <v>193</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="5"/>
     </row>
@@ -1226,16 +1235,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="F6" s="5"/>
     </row>
@@ -1244,16 +1253,16 @@
         <v>1</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>154</v>
+        <v>62</v>
       </c>
       <c r="F7" s="5"/>
     </row>
@@ -1262,16 +1271,16 @@
         <v>1</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>12</v>
+        <v>150</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>57</v>
+        <v>155</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -1280,129 +1289,131 @@
         <v>1</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>4</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>116</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>52</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
-        <v>2</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="10" t="s">
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>52</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
+      <c r="D15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>2</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>25</v>
+        <v>128</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1412,13 +1423,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
@@ -1428,13 +1439,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>129</v>
+        <v>26</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1444,13 +1455,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -1460,13 +1471,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1476,13 +1487,13 @@
         <v>2</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -1492,45 +1503,45 @@
         <v>2</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="10">
         <v>2</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="5" t="s">
+      <c r="B23" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="D23" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>162</v>
+        <v>50</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1540,160 +1551,159 @@
         <v>1</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>163</v>
+        <v>49</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>5</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>149</v>
+        <v>163</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>157</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="E29" s="5"/>
+        <v>156</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>157</v>
+      </c>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>164</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>41</v>
+        <v>164</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>2</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D33" s="6" t="s">
-        <v>183</v>
+      <c r="D33" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>2</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>172</v>
+      <c r="D34" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1701,121 +1711,122 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>90</v>
+        <v>37</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="G36" s="9"/>
+        <v>126</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>151</v>
+        <v>89</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
+        <v>171</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>140</v>
+        <v>84</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>186</v>
+        <v>80</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>65</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D41" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E41" s="5"/>
+      <c r="D41" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,52 +1834,50 @@
         <v>2</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>87</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>2</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>153</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="F43" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>91</v>
+        <v>152</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="F44" s="5"/>
     </row>
@@ -1877,15 +1886,17 @@
         <v>1</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" s="5"/>
+        <v>189</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>190</v>
+      </c>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -1893,13 +1904,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -1909,206 +1920,222 @@
         <v>1</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E47" s="5"/>
-      <c r="F47" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>165</v>
+        <v>97</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>166</v>
+        <v>98</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>99</v>
+        <v>168</v>
       </c>
       <c r="E50" s="5"/>
-      <c r="F50" s="5" t="s">
-        <v>87</v>
-      </c>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
+        <v>3</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
         <v>1</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B52" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D52" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>105</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" t="s">
-        <v>134</v>
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C58" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>110</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>139</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
-    </row>
-    <row r="69" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="70" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>178</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>180</v>
       </c>
     </row>

</xml_diff>